<commit_message>
Test data for Spain added
</commit_message>
<xml_diff>
--- a/Test Data/FC_Gallery_AttachedFunctionality_FIM_Node.xlsx
+++ b/Test Data/FC_Gallery_AttachedFunctionality_FIM_Node.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297CB512-5696-480B-AB51-C76F1B14DC92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F56E9E-B72D-40B6-AEC8-974E706D322A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Italy" sheetId="16" r:id="rId1"/>
+    <sheet name="Spain" sheetId="17" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Wg</t>
   </si>
@@ -72,6 +73,12 @@
   </si>
   <si>
     <t>NGC-3443/T1931/T1941</t>
+  </si>
+  <si>
+    <t>Spain Market</t>
+  </si>
+  <si>
+    <t>NGC-3442/T1602/T1643</t>
   </si>
 </sst>
 </file>
@@ -495,6 +502,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EEBBF9-A001-4704-AEF0-91633C1E4D79}">
   <dimension ref="A1:D10"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D5A652-AB3A-4112-9E5F-6FA6329859D8}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -520,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -542,7 +646,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>

<commit_message>
Added UK FC market test cases added
</commit_message>
<xml_diff>
--- a/Test Data/FC_Gallery_AttachedFunctionality_FIM_Node.xlsx
+++ b/Test Data/FC_Gallery_AttachedFunctionality_FIM_Node.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D90BC4C-0A79-4807-A37D-A6F57ABA2377}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856442C2-C3D4-4CD6-90EF-C27312227E3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Italy" sheetId="16" r:id="rId1"/>
-    <sheet name="Spain" sheetId="17" r:id="rId2"/>
-    <sheet name="Hungary" sheetId="18" r:id="rId3"/>
+    <sheet name="UK" sheetId="19" r:id="rId1"/>
+    <sheet name="Italy" sheetId="16" r:id="rId2"/>
+    <sheet name="Spain" sheetId="17" r:id="rId3"/>
+    <sheet name="Hungary" sheetId="18" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>Wg</t>
   </si>
@@ -86,6 +87,12 @@
   </si>
   <si>
     <t>NGC-4308/T3626/T3644</t>
+  </si>
+  <si>
+    <t>UK Market</t>
+  </si>
+  <si>
+    <t>NGC-3003/T1251/T1260</t>
   </si>
 </sst>
 </file>
@@ -506,6 +513,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71FC657-2EFE-42D6-92F7-E7CC78F2F346}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EEBBF9-A001-4704-AEF0-91633C1E4D79}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -602,7 +706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D5A652-AB3A-4112-9E5F-6FA6329859D8}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -699,12 +803,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3E7DDA-5C3C-4C90-9A52-5147B07D2B6B}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>